<commit_message>
7 cmt done import thuoc
</commit_message>
<xml_diff>
--- a/TMTDentalAPI/ClientApp/src/assets/files/MauFileThuoc.xlsx
+++ b/TMTDentalAPI/ClientApp/src/assets/files/MauFileThuoc.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GIGA\Documents\Projects\TDental\TMTDentalAPI\ClientApp\src\assets\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I710700\Desktop\Source\TDental\TMTDentalAPI\ClientApp\src\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Tên thuốc</t>
   </si>
@@ -36,6 +36,15 @@
   </si>
   <si>
     <t>Thuốc giảm đau</t>
+  </si>
+  <si>
+    <t>Giá thuốc</t>
+  </si>
+  <si>
+    <t>Đơn vị mặc định</t>
+  </si>
+  <si>
+    <t>cái</t>
   </si>
 </sst>
 </file>
@@ -79,9 +88,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -362,32 +373,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="2"/>
+    <col min="4" max="4" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
+      </c>
+      <c r="C2" s="2">
+        <v>100000</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>